<commit_message>
Refactor code, DLL support, composite frame as inputblock support, paraEventsOnly parameter added, new plot framework
</commit_message>
<xml_diff>
--- a/Powerfactory/TestCases.xlsx
+++ b/Powerfactory/TestCases.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKT.ENERGINET\Desktop\PP-MTB-Alpha\PP-MTB PSCAD\DK1_DSO_D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MKT.ENERGINET\Desktop\PP-MTB-Git\PP-MTB Powerfactory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="350"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="350" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="151">
   <si>
     <t>PrefCtrl</t>
   </si>
@@ -559,7 +559,13 @@
     <t>Included</t>
   </si>
   <si>
-    <t>Fredericia</t>
+    <t>Aadum</t>
+  </si>
+  <si>
+    <t>3.9.9.9</t>
+  </si>
+  <si>
+    <t>PF_test</t>
   </si>
 </sst>
 </file>
@@ -1261,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,28 +1334,28 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="15">
-        <v>10</v>
+        <v>37.567999999999998</v>
       </c>
       <c r="C2" s="15">
-        <v>10</v>
+        <v>37.567999999999998</v>
       </c>
       <c r="D2" s="15">
         <v>62.5</v>
       </c>
       <c r="E2" s="15">
+        <v>10.520333333333333</v>
+      </c>
+      <c r="F2" s="15">
+        <v>2.7475000000000001</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
         <v>5</v>
       </c>
-      <c r="F2" s="15">
-        <v>15</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
       <c r="I2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J2" t="s">
         <v>148</v>
@@ -1425,9 +1431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK24" sqref="AK24"/>
+      <selection pane="bottomLeft" activeCell="AB25" sqref="AB25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1597,7 +1603,7 @@
       </c>
       <c r="F2" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G2" s="25">
         <v>0</v>
@@ -1714,7 +1720,7 @@
       </c>
       <c r="F3" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G3" s="25">
         <v>0</v>
@@ -1831,7 +1837,7 @@
       </c>
       <c r="F4" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G4" s="25">
         <v>0</v>
@@ -1948,7 +1954,7 @@
       </c>
       <c r="F5" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G5" s="25">
         <v>0</v>
@@ -2065,7 +2071,7 @@
       </c>
       <c r="F6" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G6" s="25">
         <v>0</v>
@@ -2182,7 +2188,7 @@
       </c>
       <c r="F7" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7" s="25">
         <v>0</v>
@@ -2299,7 +2305,7 @@
       </c>
       <c r="F8" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G8" s="25">
         <v>0</v>
@@ -2416,7 +2422,7 @@
       </c>
       <c r="F9" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G9" s="25">
         <v>0</v>
@@ -2533,7 +2539,7 @@
       </c>
       <c r="F10" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G10" s="25">
         <v>0</v>
@@ -2650,7 +2656,7 @@
       </c>
       <c r="F11" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G11" s="25">
         <v>0</v>
@@ -2767,7 +2773,7 @@
       </c>
       <c r="F12" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G12" s="25">
         <v>0</v>
@@ -2884,7 +2890,7 @@
       </c>
       <c r="F13" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G13" s="25">
         <v>0</v>
@@ -3001,7 +3007,7 @@
       </c>
       <c r="F14" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G14" s="25">
         <v>0</v>
@@ -3118,7 +3124,7 @@
       </c>
       <c r="F15" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G15" s="25">
         <v>0</v>
@@ -3235,7 +3241,7 @@
       </c>
       <c r="F16" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G16" s="25">
         <v>0</v>
@@ -3352,7 +3358,7 @@
       </c>
       <c r="F17" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G17" s="25">
         <v>0</v>
@@ -3469,7 +3475,7 @@
       </c>
       <c r="F18" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G18" s="25">
         <v>0</v>
@@ -3586,7 +3592,7 @@
       </c>
       <c r="F19" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G19" s="25">
         <v>0</v>
@@ -3703,7 +3709,7 @@
       </c>
       <c r="F20" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20" s="25">
         <v>0</v>
@@ -3820,7 +3826,7 @@
       </c>
       <c r="F21" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G21" s="25">
         <v>-0.33</v>
@@ -3937,7 +3943,7 @@
       </c>
       <c r="F22" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G22" s="25">
         <v>0.33</v>
@@ -4054,7 +4060,7 @@
       </c>
       <c r="F23" s="29">
         <f>Input!H2</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G23" s="25">
         <v>1</v>
@@ -4094,7 +4100,7 @@
       </c>
       <c r="S23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.025</f>
-        <v>1.0316739272428239</v>
+        <v>0.99660432189671699</v>
       </c>
       <c r="T23" s="1">
         <v>0</v>
@@ -4104,7 +4110,7 @@
       </c>
       <c r="V23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) - 0.025</f>
-        <v>0.98167392724282398</v>
+        <v>0.94660432189671695</v>
       </c>
       <c r="W23" s="1">
         <v>0</v>
@@ -4114,7 +4120,7 @@
       </c>
       <c r="Y23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
-        <v>1.006673927242824</v>
+        <v>0.97160432189671697</v>
       </c>
       <c r="Z23" s="1">
         <v>0</v>
@@ -4124,7 +4130,7 @@
       </c>
       <c r="AB23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.05</f>
-        <v>1.0566739272428241</v>
+        <v>1.021604321896717</v>
       </c>
       <c r="AC23" s="1">
         <v>0</v>
@@ -4134,7 +4140,7 @@
       </c>
       <c r="AE23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
-        <v>1.006673927242824</v>
+        <v>0.97160432189671697</v>
       </c>
       <c r="AF23" s="4">
         <v>0</v>
@@ -4144,7 +4150,7 @@
       </c>
       <c r="AH23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) - 0.05</f>
-        <v>0.95667392724282396</v>
+        <v>0.92160432189671693</v>
       </c>
       <c r="AI23" s="1">
         <v>0</v>
@@ -4154,7 +4160,7 @@
       </c>
       <c r="AK23" s="34">
         <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2)</f>
-        <v>1.006673927242824</v>
+        <v>0.97160432189671697</v>
       </c>
       <c r="AL23" s="1">
         <v>0</v>
@@ -4178,7 +4184,7 @@
       </c>
       <c r="F24" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G24" s="25">
         <v>0</v>
@@ -4295,7 +4301,7 @@
       </c>
       <c r="F25" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G25" s="25">
         <v>0</v>
@@ -4393,10 +4399,7 @@
       <c r="AL25" s="3">
         <v>0</v>
       </c>
-      <c r="AQ25" s="34">
-        <f>SQRT((1 - Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1))^2 +  (Cases!$E$23/Input!$E$2/SQRT(Input!$F$2*Input!$F$2+1) * Input!$F$2)^2) + 0.025</f>
-        <v>1.0316739272428239</v>
-      </c>
+      <c r="AQ25" s="34"/>
     </row>
     <row r="26" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -4416,7 +4419,7 @@
       </c>
       <c r="F26" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G26" s="25">
         <v>0</v>
@@ -4533,7 +4536,7 @@
       </c>
       <c r="F27" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G27" s="25">
         <v>0</v>
@@ -4650,7 +4653,7 @@
       </c>
       <c r="F28" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G28" s="25">
         <v>0</v>
@@ -4767,7 +4770,7 @@
       </c>
       <c r="F29" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G29" s="25">
         <v>0</v>
@@ -4884,7 +4887,7 @@
       </c>
       <c r="F30" s="29">
         <f>Input!I2</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G30" s="25">
         <v>0.99</v>
@@ -5001,7 +5004,7 @@
       </c>
       <c r="F31" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G31" s="25">
         <v>0</v>
@@ -5118,7 +5121,7 @@
       </c>
       <c r="F32" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G32" s="25">
         <v>0</v>
@@ -5235,7 +5238,7 @@
       </c>
       <c r="F33" s="26">
         <f>Input!G2</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G33" s="25">
         <v>0</v>
@@ -5331,6 +5334,123 @@
         <v>0</v>
       </c>
       <c r="AL33" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="1">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="29">
+        <f>Input!I2</f>
+        <v>6</v>
+      </c>
+      <c r="G34" s="1">
+        <v>1</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <v>1</v>
+      </c>
+      <c r="J34" s="1">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0</v>
+      </c>
+      <c r="L34" s="1">
+        <v>0</v>
+      </c>
+      <c r="M34" s="1">
+        <v>0</v>
+      </c>
+      <c r="N34" s="1">
+        <v>0</v>
+      </c>
+      <c r="O34" s="1">
+        <v>0</v>
+      </c>
+      <c r="P34" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>20</v>
+      </c>
+      <c r="R34" s="1">
+        <v>3</v>
+      </c>
+      <c r="S34" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="T34" s="1">
+        <v>0</v>
+      </c>
+      <c r="U34" s="1">
+        <v>10</v>
+      </c>
+      <c r="V34" s="1">
+        <v>-0.9</v>
+      </c>
+      <c r="W34" s="1">
+        <v>0</v>
+      </c>
+      <c r="X34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="1">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AF34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AG34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AI34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>